<commit_message>
remove zips with two leading zeros in fake data
</commit_message>
<xml_diff>
--- a/cardExchangeFakeData.xlsx
+++ b/cardExchangeFakeData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julie/dev2/code_signal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julie/dev2/card_exchanges/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CB9681-39E1-DA48-9F26-05BE3E8659E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B34DA43-BF25-174B-91DF-A2C465BD0296}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="500" windowWidth="24980" windowHeight="16100" xr2:uid="{D9246678-8E6C-8A49-9E09-323E05E01436}"/>
+    <workbookView xWindow="1560" yWindow="500" windowWidth="24980" windowHeight="16100" xr2:uid="{D9246678-8E6C-8A49-9E09-323E05E01436}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -669,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66F453D-BAC9-FB45-A8DB-8EB591CDB891}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -963,7 +963,7 @@
         <v>69</v>
       </c>
       <c r="K8">
-        <v>234</v>
+        <v>2342</v>
       </c>
       <c r="L8" s="3"/>
     </row>
@@ -1125,7 +1125,7 @@
         <v>69</v>
       </c>
       <c r="K14">
-        <v>234</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="15" spans="1:15">

</xml_diff>